<commit_message>
Add more grocery stores and convert excel to a csv file
</commit_message>
<xml_diff>
--- a/grocery stores.xlsx
+++ b/grocery stores.xlsx
@@ -1,36 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Navi\Documents\School\CS 438 (Big Data)\LetsGetThisBread\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4ADDDC62-6DC5-4C68-B10B-89ADAFA93DC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B6CE94C-0A71-4F0F-89DF-DE91FE863490}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6705" xr2:uid="{12EF42C5-9ED1-485F-8618-38F9613D739F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="73">
   <si>
     <t>Grocery Store Name</t>
   </si>
@@ -62,43 +52,193 @@
     <t>1210 NW Couch St, Portland, OR 97209</t>
   </si>
   <si>
+    <t>New Seasons</t>
+  </si>
+  <si>
+    <t>University Park, 6300 N Lombard St, Portland, OR 97203</t>
+  </si>
+  <si>
+    <t>New Seasons Market Arbor Lodge, 6400 N Interstate Ave, Portland, OR 97217</t>
+  </si>
+  <si>
+    <t>2170 NW Raleigh St, Portland, OR 97210</t>
+  </si>
+  <si>
+    <t>3445 N Williams Ave, Portland, OR 97212</t>
+  </si>
+  <si>
+    <t>5320 NE 33rd Ave, Portland, OR 97211</t>
+  </si>
+  <si>
+    <t>3210 NE Broadway St, Portland, OR 97232</t>
+  </si>
+  <si>
+    <t>4034 SE Hawthorne Blvd, Portland, OR 97214</t>
+  </si>
+  <si>
+    <t>1954 SE Division St, Portland, OR 97202</t>
+  </si>
+  <si>
+    <t>4500 SE Woodstock Blvd, Portland, OR 97206</t>
+  </si>
+  <si>
+    <t>1214 SE Tacoma St, Portland, OR 97202</t>
+  </si>
+  <si>
+    <t>Walmart</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>1123 N Hayden Meadows Dr, Portland, OR 97217</t>
+  </si>
+  <si>
+    <t>4200 SE 82nd Ave, Portland, OR 97266</t>
+  </si>
+  <si>
+    <t>23500 NE Sandy Blvd, Wood Village, OR 97060</t>
+  </si>
+  <si>
+    <t>Grocery Outlet</t>
+  </si>
+  <si>
+    <t>7741 N Lombard St, Portland, OR 97203</t>
+  </si>
+  <si>
+    <t>4420 NE Hancock St, Portland, OR 97213</t>
+  </si>
+  <si>
+    <t>7120 SE Flavel St, Portland, OR 97206</t>
+  </si>
+  <si>
+    <t>12102 SE Division St, Portland, OR 97266</t>
+  </si>
+  <si>
+    <t>10721 NE Sandy Blvd, Portland, OR 97220</t>
+  </si>
+  <si>
+    <t>2925 NW Division St, Gresham, OR 97030</t>
+  </si>
+  <si>
+    <t>Green Zebra</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>3011 N Lombard St, Portland, OR 97217</t>
+  </si>
+  <si>
+    <t>1704 SW Broadway, Portland, OR 97201</t>
+  </si>
+  <si>
+    <t>808 NE Multnomah St, Portland, OR 97232</t>
+  </si>
+  <si>
+    <t>Fred Meyer</t>
+  </si>
+  <si>
+    <t>6850 N Lombard St, Portland, OR 97203</t>
+  </si>
+  <si>
+    <t>7404 N Interstate Ave, Portland, OR 97217</t>
+  </si>
+  <si>
+    <t>100 NW 20th Pl, Portland, OR 97209</t>
+  </si>
+  <si>
+    <t>3030 NE Weidler St, Portland, OR 97232</t>
+  </si>
+  <si>
+    <t>7555 SW Barbur Blvd, Portland, OR 97219</t>
+  </si>
+  <si>
+    <t>3805 SE Hawthorne Blvd, Portland, OR 97214</t>
+  </si>
+  <si>
+    <t>6615 NE Glisan St, Portland, OR 97213</t>
+  </si>
+  <si>
+    <t>1111 NE 102nd Ave, Portland, OR 97220</t>
+  </si>
+  <si>
+    <t>14700 SE Division St, Portland, OR 97236</t>
+  </si>
+  <si>
+    <t>22855 NE Park Ln, Wood Village, OR 97060</t>
+  </si>
+  <si>
+    <t>Safeway</t>
+  </si>
+  <si>
+    <t>8330 N Ivanhoe St, Portland, OR 97203</t>
+  </si>
+  <si>
+    <t>5920 NE Martin Luther King Jr Blvd, Portland, OR 97211</t>
+  </si>
+  <si>
+    <t>6901 NE Sandy Blvd, Portland, OR 97213</t>
+  </si>
+  <si>
+    <t>1100 NE Broadway St, Portland, OR 97232</t>
+  </si>
+  <si>
+    <t>1303 NW Lovejoy St, Portland, OR 97209</t>
+  </si>
+  <si>
+    <t>1010 SW Jefferson St, Portland, OR 97201</t>
+  </si>
+  <si>
+    <t>2800 SE Hawthorne Blvd, Portland, OR 97214</t>
+  </si>
+  <si>
+    <t>3930 SE Powell Blvd, Portland, OR 97202</t>
+  </si>
+  <si>
+    <t>4515 SE Woodstock Blvd, Portland, OR 97206</t>
+  </si>
+  <si>
+    <t>8145 SW Barbur Blvd, Portland, OR 97219</t>
+  </si>
+  <si>
+    <t>3527 SE 122nd Ave, Portland, OR 97236</t>
+  </si>
+  <si>
+    <t>1001 SW Highland Dr, Gresham, OR 97080</t>
+  </si>
+  <si>
+    <t>1455 NE Division St, Gresham, OR 97030</t>
+  </si>
+  <si>
+    <t>2501 SW Cherry Park Rd, Troutdale, OR 97060</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>1555 N Tomahawk Island Dr, Portland, OR 97217</t>
+  </si>
+  <si>
+    <t>939 SW Morrison St, Portland, OR 97205</t>
+  </si>
+  <si>
+    <t>9401 NE Cascades Pkwy, Portland, OR 97220</t>
+  </si>
+  <si>
+    <t>3031 SE Powell Blvd, Portland, OR 97202</t>
+  </si>
+  <si>
+    <t>9800 SE Washington St, Portland, OR 97216</t>
+  </si>
+  <si>
+    <t>21500 NE Halsey St, Fairview, OR 97024</t>
+  </si>
+  <si>
+    <t>Resources</t>
+  </si>
+  <si>
     <t>http://ciclt.net/sn/clt/capitolimpact/gw_ziplist.aspx?ClientCode=capitolimpact&amp;State=or&amp;StName=Oregon&amp;StFIPS=41&amp;FIPS=41051</t>
-  </si>
-  <si>
-    <t>Resources</t>
-  </si>
-  <si>
-    <t>University Park, 6300 N Lombard St, Portland, OR 97203</t>
-  </si>
-  <si>
-    <t>New Seasons</t>
-  </si>
-  <si>
-    <t>New Seasons Market Arbor Lodge, 6400 N Interstate Ave, Portland, OR 97217</t>
-  </si>
-  <si>
-    <t>2170 NW Raleigh St, Portland, OR 97210</t>
-  </si>
-  <si>
-    <t>3445 N Williams Ave, Portland, OR 97212</t>
-  </si>
-  <si>
-    <t>5320 NE 33rd Ave, Portland, OR 97211</t>
-  </si>
-  <si>
-    <t>3210 NE Broadway St, Portland, OR 97232</t>
-  </si>
-  <si>
-    <t>4034 SE Hawthorne Blvd, Portland, OR 97214</t>
-  </si>
-  <si>
-    <t>1954 SE Division St, Portland, OR 97202</t>
-  </si>
-  <si>
-    <t>4500 SE Woodstock Blvd, Portland, OR 97206</t>
-  </si>
-  <si>
-    <t>1214 SE Tacoma St, Portland, OR 97202</t>
   </si>
 </sst>
 </file>
@@ -181,7 +321,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -193,7 +333,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -240,23 +380,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -292,23 +415,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -460,11 +566,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1B2B03E-CF8B-4911-8182-47508D5A1463}">
-  <dimension ref="A1:F15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="F1" sqref="F1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -483,7 +589,7 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
@@ -500,7 +606,7 @@
         <v>97212</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>10</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -547,13 +653,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6">
         <v>97203</v>
@@ -561,13 +667,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D7">
         <v>97217</v>
@@ -575,13 +681,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D8">
         <v>97210</v>
@@ -589,13 +695,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D9">
         <v>97212</v>
@@ -603,13 +709,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D10">
         <v>97211</v>
@@ -617,13 +723,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D11">
         <v>97232</v>
@@ -631,13 +737,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D12">
         <v>97214</v>
@@ -645,13 +751,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D13">
         <v>97202</v>
@@ -659,13 +765,13 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D14">
         <v>97206</v>
@@ -673,21 +779,609 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D15">
         <v>97202</v>
       </c>
     </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16">
+        <v>97217</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17">
+        <v>97266</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18">
+        <v>97060</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19">
+        <v>97203</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20">
+        <v>97213</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21">
+        <v>97206</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22">
+        <v>97266</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23">
+        <v>97220</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24">
+        <v>97030</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25">
+        <v>97217</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26">
+        <v>97201</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27">
+        <v>97232</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28">
+        <v>97203</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29">
+        <v>97217</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30">
+        <v>97209</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31">
+        <v>97232</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32">
+        <v>97219</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33">
+        <v>97214</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34">
+        <v>97213</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35">
+        <v>97220</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" t="s">
+        <v>47</v>
+      </c>
+      <c r="D36">
+        <v>97236</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37">
+        <v>97060</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" t="s">
+        <v>34</v>
+      </c>
+      <c r="C38" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38">
+        <v>97203</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" t="s">
+        <v>51</v>
+      </c>
+      <c r="D39">
+        <v>97211</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" t="s">
+        <v>34</v>
+      </c>
+      <c r="C40" t="s">
+        <v>52</v>
+      </c>
+      <c r="D40">
+        <v>97213</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>49</v>
+      </c>
+      <c r="B41" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41" t="s">
+        <v>53</v>
+      </c>
+      <c r="D41">
+        <v>97232</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" t="s">
+        <v>54</v>
+      </c>
+      <c r="D42">
+        <v>97209</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43" t="s">
+        <v>34</v>
+      </c>
+      <c r="C43" t="s">
+        <v>55</v>
+      </c>
+      <c r="D43">
+        <v>97201</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" t="s">
+        <v>34</v>
+      </c>
+      <c r="C44" t="s">
+        <v>56</v>
+      </c>
+      <c r="D44">
+        <v>97214</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45" t="s">
+        <v>34</v>
+      </c>
+      <c r="C45" t="s">
+        <v>57</v>
+      </c>
+      <c r="D45">
+        <v>97202</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46" t="s">
+        <v>34</v>
+      </c>
+      <c r="C46" t="s">
+        <v>58</v>
+      </c>
+      <c r="D46">
+        <v>97206</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47" t="s">
+        <v>34</v>
+      </c>
+      <c r="C47" t="s">
+        <v>59</v>
+      </c>
+      <c r="D47">
+        <v>97219</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48" t="s">
+        <v>34</v>
+      </c>
+      <c r="C48" t="s">
+        <v>60</v>
+      </c>
+      <c r="D48">
+        <v>97236</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" t="s">
+        <v>34</v>
+      </c>
+      <c r="C49" t="s">
+        <v>61</v>
+      </c>
+      <c r="D49">
+        <v>97080</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>34</v>
+      </c>
+      <c r="C50" t="s">
+        <v>62</v>
+      </c>
+      <c r="D50">
+        <v>97030</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>34</v>
+      </c>
+      <c r="C51" t="s">
+        <v>63</v>
+      </c>
+      <c r="D51">
+        <v>97060</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
+        <v>64</v>
+      </c>
+      <c r="B52" t="s">
+        <v>34</v>
+      </c>
+      <c r="C52" t="s">
+        <v>65</v>
+      </c>
+      <c r="D52">
+        <v>97217</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
+        <v>64</v>
+      </c>
+      <c r="B53" t="s">
+        <v>34</v>
+      </c>
+      <c r="C53" t="s">
+        <v>66</v>
+      </c>
+      <c r="D53">
+        <v>97205</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A54" t="s">
+        <v>64</v>
+      </c>
+      <c r="B54" t="s">
+        <v>34</v>
+      </c>
+      <c r="C54" t="s">
+        <v>67</v>
+      </c>
+      <c r="D54">
+        <v>97220</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
+        <v>64</v>
+      </c>
+      <c r="B55" t="s">
+        <v>34</v>
+      </c>
+      <c r="C55" t="s">
+        <v>68</v>
+      </c>
+      <c r="D55">
+        <v>97202</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
+        <v>64</v>
+      </c>
+      <c r="B56" t="s">
+        <v>34</v>
+      </c>
+      <c r="C56" t="s">
+        <v>69</v>
+      </c>
+      <c r="D56">
+        <v>97216</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
+        <v>64</v>
+      </c>
+      <c r="B57" t="s">
+        <v>34</v>
+      </c>
+      <c r="C57" t="s">
+        <v>70</v>
+      </c>
+      <c r="D57">
+        <v>97024</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{0969D0B1-BCD0-4A0E-8802-52B6990D54E4}"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{6F275A5B-1A55-4BE3-AF39-2BF33C8F6487}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>